<commit_message>
Expanding readme and sample data
</commit_message>
<xml_diff>
--- a/Sample Data.xlsx
+++ b/Sample Data.xlsx
@@ -4,11 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="16900" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,12 +18,143 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="34">
+  <si>
+    <t>Berklee ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Bob Kelso</t>
+  </si>
+  <si>
+    <t>Bruce Wayne</t>
+  </si>
+  <si>
+    <t>Edward Meechum</t>
+  </si>
+  <si>
+    <t>Jessica Jones</t>
+  </si>
+  <si>
+    <t>Mark Twain</t>
+  </si>
+  <si>
+    <t>Rock Strongo</t>
+  </si>
+  <si>
+    <t>Tom Ashbrook</t>
+  </si>
+  <si>
+    <t>Condoleeza Rice</t>
+  </si>
+  <si>
+    <t>Donella Meadows</t>
+  </si>
+  <si>
+    <t>Michel Foucault</t>
+  </si>
+  <si>
+    <t>Program</t>
+  </si>
+  <si>
+    <t>BM4.UNDL</t>
+  </si>
+  <si>
+    <t>PDM.UNDL</t>
+  </si>
+  <si>
+    <t>SNM.POST</t>
+  </si>
+  <si>
+    <t>Credits Enrolled</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>FT</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t>0360009</t>
+  </si>
+  <si>
+    <t>0213906</t>
+  </si>
+  <si>
+    <t>0770027</t>
+  </si>
+  <si>
+    <t>0480151</t>
+  </si>
+  <si>
+    <t>0139531</t>
+  </si>
+  <si>
+    <t>0965643</t>
+  </si>
+  <si>
+    <t>0626394</t>
+  </si>
+  <si>
+    <t>0900882</t>
+  </si>
+  <si>
+    <t>0590486</t>
+  </si>
+  <si>
+    <t>0471104</t>
+  </si>
+  <si>
+    <t>Data Columns</t>
+  </si>
+  <si>
+    <t>Challenge Columns</t>
+  </si>
+  <si>
+    <t>1-a</t>
+  </si>
+  <si>
+    <t>1-b</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -47,13 +177,41 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="13">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -383,30 +541,235 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="15.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="2">
+        <v>2</v>
+      </c>
+      <c r="I2" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12">
+        <v>6</v>
+      </c>
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <ignoredErrors>
+    <ignoredError sqref="A3:A12" numberStoredAsText="1"/>
+  </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
removed "Credits Enrolled" field for now
</commit_message>
<xml_diff>
--- a/Sample Data.xlsx
+++ b/Sample Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="35700" yWindow="-6920" windowWidth="25600" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="33220" yWindow="-7680" windowWidth="25600" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="122">
   <si>
     <t>Berklee ID</t>
   </si>
@@ -68,9 +68,6 @@
   </si>
   <si>
     <t>SNM.POST</t>
-  </si>
-  <si>
-    <t>Credits Enrolled</t>
   </si>
   <si>
     <t>Status</t>
@@ -844,10 +841,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -855,12 +852,11 @@
     <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1">
+    <row r="1" spans="1:8" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -873,17 +869,14 @@
       <c r="D1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="E1"/>
       <c r="F1"/>
-      <c r="G1"/>
+      <c r="G1" s="2"/>
       <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-    </row>
-    <row r="2" spans="1:9">
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -891,16 +884,13 @@
       <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -908,16 +898,13 @@
       <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="D3">
-        <v>15</v>
-      </c>
-      <c r="E3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -925,50 +912,41 @@
       <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="D4">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6">
-        <v>9</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -976,16 +954,13 @@
       <c r="C7" t="s">
         <v>13</v>
       </c>
-      <c r="D7">
-        <v>4</v>
-      </c>
-      <c r="E7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
@@ -993,16 +968,13 @@
       <c r="C8" t="s">
         <v>14</v>
       </c>
-      <c r="D8">
-        <v>4</v>
-      </c>
-      <c r="E8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -1010,16 +982,13 @@
       <c r="C9" t="s">
         <v>13</v>
       </c>
-      <c r="D9">
-        <v>3</v>
-      </c>
-      <c r="E9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
@@ -1027,16 +996,13 @@
       <c r="C10" t="s">
         <v>13</v>
       </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-      <c r="E10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -1044,11 +1010,8 @@
       <c r="C11" t="s">
         <v>15</v>
       </c>
-      <c r="D11">
-        <v>6</v>
-      </c>
-      <c r="E11" t="s">
-        <v>19</v>
+      <c r="D11" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1083,368 +1046,368 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>112</v>
-      </c>
       <c r="D1" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>114</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>118</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>